<commit_message>
Added the positions to the numbers and letters
</commit_message>
<xml_diff>
--- a/documents/Dimensionen.xlsx
+++ b/documents/Dimensionen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MP107\Documents\car-dash-MC\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CEA671D-ECF0-443B-9851-416A5F8E4D4B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{733ECEE8-7183-49E1-84C7-29CC6A81BF14}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3660" yWindow="2370" windowWidth="14400" windowHeight="7360" xr2:uid="{EC7381E9-354D-422F-9E09-F97A0B045F03}"/>
   </bookViews>
@@ -54,9 +54,6 @@
     <t>Real</t>
   </si>
   <si>
-    <t>Letters</t>
-  </si>
-  <si>
     <t>Bezeichner</t>
   </si>
   <si>
@@ -64,6 +61,9 @@
   </si>
   <si>
     <t>Anzahl</t>
+  </si>
+  <si>
+    <t>Direction</t>
   </si>
 </sst>
 </file>
@@ -459,8 +459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13E2847E-3ADB-4FF2-84EF-A7CD0F6BCED5}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -510,7 +510,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1">
         <f>D6*B6</f>
@@ -529,7 +529,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -586,7 +586,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -613,13 +613,13 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>1</v>
       </c>
       <c r="I16" s="1">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -636,14 +636,14 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1">
         <f>I16*G16</f>
-        <v>2016</v>
+        <v>1161</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>